<commit_message>
ALP Costing Complete with Requisition , User Allocation , Department Allocation , Emailing , ALP Costing Payroll , User Allocation Billing
ALL done
</commit_message>
<xml_diff>
--- a/Web/Template/Excel/ALP_Costing_Sheet.xlsx
+++ b/Web/Template/Excel/ALP_Costing_Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohail.ahmed\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SohailWorkspace\CorporateAndFinanceProject\Solution\CorporateAndFinance\Web\Template\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -202,7 +202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -214,6 +214,10 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,13 +502,14 @@
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="18" style="5" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
@@ -529,7 +534,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -580,6 +585,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>